<commit_message>
Removed unnecessary comments and updated readme file
</commit_message>
<xml_diff>
--- a/code/src/backend/temp/violations_output.xlsx
+++ b/code/src/backend/temp/violations_output.xlsx
@@ -151,14 +151,14 @@
   <commentList>
     <comment ref="A2" authorId="0" shapeId="0">
       <text>
-        <t>Violation: Invalid format, contains a decimal and is not a string.
-Remediation: Remove the decimal and convert to string.</t>
+        <t>Violation: Invalid format, contains a decimal and exceeds the maximum value of 50.
+Remediation: Remove the decimal, convert to an integer, and ensure it's less than 50.</t>
       </text>
     </comment>
     <comment ref="E2" authorId="0" shapeId="0">
       <text>
-        <t>Violation: Invalid format, should be a 2-letter ISO 3166-1 alpha-2 code.
-Remediation: Correct the country code to a valid ISO 3166-1 alpha-2 code.</t>
+        <t>Violation: Invalid format, must be a valid two-letter ISO 3166-1 alpha-2 code.
+Remediation: Correct the country code to a valid two-letter ISO 3166-1 alpha-2 code.</t>
       </text>
     </comment>
     <comment ref="F2" authorId="0" shapeId="0">
@@ -179,6 +179,24 @@
 Remediation: Ensure the format matches the requirements.</t>
       </text>
     </comment>
+    <comment ref="M2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, needs to be yyyy-mm-dd.
+Remediation: Convert to yyyy-mm-dd format.</t>
+      </text>
+    </comment>
+    <comment ref="Q2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="R2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
     <comment ref="S2" authorId="0" shapeId="0">
       <text>
         <t>Violation: Invalid format, should be a decimal.
@@ -187,20 +205,68 @@
     </comment>
     <comment ref="T2" authorId="0" shapeId="0">
       <text>
-        <t>Violation: Invalid format, should be an integer based on the predefined codes.
+        <t>Violation: Invalid format, should be an integer.
 Remediation: Convert to integer based on the predefined codes.</t>
       </text>
     </comment>
     <comment ref="Y2" authorId="0" shapeId="0">
       <text>
-        <t>Violation: Invalid format, should be an integer based on the predefined codes.
+        <t>Violation: Invalid format, should be an integer.
 Remediation: Convert to integer based on the predefined codes.</t>
       </text>
     </comment>
+    <comment ref="Z2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="AF2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AG2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AH2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AI2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AJ2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AK2" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
     <comment ref="A3" authorId="0" shapeId="0">
       <text>
-        <t>Violation: Invalid format, contains a decimal and is not a string.
-Remediation: Remove the decimal and convert to string.</t>
+        <t>Violation: Invalid format, contains a decimal and exceeds the maximum value of 50.
+Remediation: Remove the decimal, convert to an integer, and ensure it's less than 50.</t>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, must be a valid two-letter ISO 3166-1 alpha-2 code.
+Remediation: Correct the country code to a valid two-letter ISO 3166-1 alpha-2 code.</t>
       </text>
     </comment>
     <comment ref="F3" authorId="0" shapeId="0">
@@ -209,154 +275,394 @@
 Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="K3" authorId="0" shapeId="0">
       <text>
         <t>Violation: Invalid format.
 Remediation: Ensure the format matches the requirements.</t>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, needs to be yyyy-mm-dd.
+Remediation: Convert to yyyy-mm-dd format.</t>
+      </text>
+    </comment>
+    <comment ref="Q3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="R3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="S3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a decimal.
+Remediation: Convert to decimal format (e.g., 0.0214).</t>
+      </text>
+    </comment>
+    <comment ref="T3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="Y3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="Z3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="AF3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AG3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AH3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AI3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AJ3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AK3" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, contains a decimal and exceeds the maximum value of 50.
+Remediation: Remove the decimal, convert to an integer, and ensure it's less than 50.</t>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, must be a valid two-letter ISO 3166-1 alpha-2 code.
+Remediation: Correct the country code to a valid two-letter ISO 3166-1 alpha-2 code.</t>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Potentially valid, requires NAICS/SIC/GICS lookup verification.
+Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
+      </text>
+    </comment>
+    <comment ref="K4" authorId="0" shapeId="0">
       <text>
         <t>Violation: Invalid format.
 Remediation: Ensure the format matches the requirements.</t>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, contains a decimal and is not a string.
-Remediation: Remove the decimal and convert to string.</t>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, should be a 2-letter ISO 3166-1 alpha-2 code.
-Remediation: Correct the country code to a valid ISO 3166-1 alpha-2 code.</t>
-      </text>
-    </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="Q4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="R4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="S4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a decimal.
+Remediation: Convert to decimal format (e.g., 0.029).</t>
+      </text>
+    </comment>
+    <comment ref="T4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="Y4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="AF4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AG4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AH4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AI4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AJ4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AK4" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, contains a decimal and exceeds the maximum value of 50.
+Remediation: Remove the decimal, convert to an integer, and ensure it's less than 50.</t>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, must be a valid two-letter ISO 3166-1 alpha-2 code.
+Remediation: Correct the country code to a valid two-letter ISO 3166-1 alpha-2 code.</t>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <t>Violation: Potentially valid, requires NAICS/SIC/GICS lookup verification.
 Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="K5" authorId="0" shapeId="0">
       <text>
         <t>Violation: Invalid format.
 Remediation: Ensure the format matches the requirements.</t>
       </text>
     </comment>
-    <comment ref="K4" authorId="0" shapeId="0">
+    <comment ref="Q5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="R5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="S5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a decimal.
+Remediation: Convert to decimal format (e.g., 0.089).</t>
+      </text>
+    </comment>
+    <comment ref="T5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="Y5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="AF5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AG5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AH5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AI5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AJ5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AK5" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, contains a decimal and exceeds the maximum value of 50.
+Remediation: Remove the decimal, convert to an integer, and ensure it's less than 50.</t>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, must be a valid two-letter ISO 3166-1 alpha-2 code.
+Remediation: Correct the country code to a valid two-letter ISO 3166-1 alpha-2 code.</t>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Potentially valid, requires NAICS/SIC/GICS lookup verification.
+Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
+      </text>
+    </comment>
+    <comment ref="K6" authorId="0" shapeId="0">
       <text>
         <t>Violation: Invalid format.
 Remediation: Ensure the format matches the requirements.</t>
       </text>
     </comment>
-    <comment ref="S4" authorId="0" shapeId="0">
+    <comment ref="Q6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="R6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="S6" authorId="0" shapeId="0">
       <text>
         <t>Violation: Invalid format, should be a decimal.
-Remediation: Convert to decimal format (e.g., 0.029).</t>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, contains a decimal and is not a string.
-Remediation: Remove the decimal and convert to string.</t>
-      </text>
-    </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, should be a 2-letter ISO 3166-1 alpha-2 code.
-Remediation: Correct the country code to a valid ISO 3166-1 alpha-2 code.</t>
-      </text>
-    </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+Remediation: Convert to decimal format (e.g., 0.1018).</t>
+      </text>
+    </comment>
+    <comment ref="T6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="Y6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="AF6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AG6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AH6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AI6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AJ6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AK6" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, contains a decimal and exceeds the maximum value of 50.
+Remediation: Remove the decimal, convert to an integer, and ensure it's less than 50.</t>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0">
       <text>
         <t>Violation: Potentially valid, requires NAICS/SIC/GICS lookup verification.
 Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H7" authorId="0" shapeId="0">
       <text>
         <t>Violation: Invalid format.
 Remediation: Ensure the format matches the requirements.</t>
       </text>
     </comment>
-    <comment ref="K5" authorId="0" shapeId="0">
+    <comment ref="K7" authorId="0" shapeId="0">
       <text>
         <t>Violation: Invalid format.
 Remediation: Ensure the format matches the requirements.</t>
       </text>
     </comment>
-    <comment ref="M5" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, should be yyyy-mm-dd.
-Remediation: Change date format to yyyy-mm-dd.</t>
-      </text>
-    </comment>
-    <comment ref="N5" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, should be yyyy-mm-dd.
-Remediation: Change date format to yyyy-mm-dd.</t>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, contains a decimal and is not a string.
-Remediation: Remove the decimal and convert to string.</t>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, should be a 2-letter ISO 3166-1 alpha-2 code.
-Remediation: Correct the country code to a valid ISO 3166-1 alpha-2 code.</t>
-      </text>
-    </comment>
-    <comment ref="F6" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Potentially valid, requires NAICS/SIC/GICS lookup verification.
-Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
-      </text>
-    </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format.
-Remediation: Ensure the format matches the requirements.</t>
-      </text>
-    </comment>
-    <comment ref="K6" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format.
-Remediation: Ensure the format matches the requirements.</t>
-      </text>
-    </comment>
-    <comment ref="A7" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, contains a decimal and is not a string.
-Remediation: Remove the decimal and convert to string.</t>
-      </text>
-    </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format, should be a 2-letter ISO 3166-1 alpha-2 code.
-Remediation: Correct the country code to a valid ISO 3166-1 alpha-2 code.</t>
-      </text>
-    </comment>
-    <comment ref="F7" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Potentially valid, requires NAICS/SIC/GICS lookup verification.
-Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
-      </text>
-    </comment>
-    <comment ref="H7" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format.
-Remediation: Ensure the format matches the requirements.</t>
-      </text>
-    </comment>
-    <comment ref="K7" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format.
-Remediation: Ensure the format matches the requirements.</t>
+    <comment ref="Q7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="R7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
       </text>
     </comment>
     <comment ref="S7" authorId="0" shapeId="0">
@@ -365,28 +671,76 @@
 Remediation: Convert to decimal format (e.g., 0.0512).</t>
       </text>
     </comment>
+    <comment ref="T7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="Y7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="AF7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AG7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AH7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AI7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AJ7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AK7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AL7" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
     <comment ref="A8" authorId="0" shapeId="0">
       <text>
-        <t>Violation: Invalid format, contains a decimal and is not a string.
-Remediation: Remove the decimal and convert to string.</t>
-      </text>
-    </comment>
-    <comment ref="F8" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Potentially valid, requires NAICS/SIC/GICS lookup verification.
-Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
-      </text>
-    </comment>
-    <comment ref="H8" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format.
-Remediation: Ensure the format matches the requirements.</t>
-      </text>
-    </comment>
-    <comment ref="K8" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format.
-Remediation: Ensure the format matches the requirements.</t>
+        <t>Violation: Invalid format, contains a decimal and exceeds the maximum value of 50.
+Remediation: Remove the decimal, convert to an integer, and ensure it's less than 50.</t>
+      </text>
+    </comment>
+    <comment ref="Q8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="R8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
       </text>
     </comment>
     <comment ref="S8" authorId="0" shapeId="0">
@@ -397,32 +751,116 @@
     </comment>
     <comment ref="T8" authorId="0" shapeId="0">
       <text>
-        <t>Violation: Invalid format, should be an integer based on the predefined codes.
+        <t>Violation: Invalid format, should be an integer.
 Remediation: Convert to integer based on the predefined codes.</t>
       </text>
     </comment>
+    <comment ref="AF8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AG8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AH8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AI8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AJ8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AK8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AL8" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
     <comment ref="A9" authorId="0" shapeId="0">
       <text>
-        <t>Violation: Invalid format, contains a decimal and is not a string.
-Remediation: Remove the decimal and convert to string.</t>
-      </text>
-    </comment>
-    <comment ref="F9" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Potentially valid, requires NAICS/SIC/GICS lookup verification.
-Remediation: Verify the code against NAICS/SIC/GICS databases.</t>
-      </text>
-    </comment>
-    <comment ref="H9" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format.
-Remediation: Ensure the format matches the requirements.</t>
-      </text>
-    </comment>
-    <comment ref="K9" authorId="0" shapeId="0">
-      <text>
-        <t>Violation: Invalid format.
-Remediation: Ensure the format matches the requirements.</t>
+        <t>Violation: Invalid format, contains a decimal and exceeds the maximum value of 50.
+Remediation: Remove the decimal, convert to an integer, and ensure it's less than 50.</t>
+      </text>
+    </comment>
+    <comment ref="Q9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="R9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="S9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a decimal.
+Remediation: Convert to decimal format (e.g., 0.018).</t>
+      </text>
+    </comment>
+    <comment ref="T9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be an integer.
+Remediation: Convert to integer based on the predefined codes.</t>
+      </text>
+    </comment>
+    <comment ref="AF9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AG9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AH9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AI9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AJ9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
+      </text>
+    </comment>
+    <comment ref="AK9" authorId="0" shapeId="0">
+      <text>
+        <t>Violation: Invalid format, should be a whole dollar amount.
+Remediation: Round to the nearest whole dollar.</t>
       </text>
     </comment>
   </commentList>
@@ -980,7 +1418,7 @@
           <t>3b531ed9-6ace-4faf-8683-85598b2e2fd2</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" s="2" t="inlineStr">
         <is>
           <t>14-08-2024</t>
         </is>
@@ -1000,10 +1438,10 @@
           <t>Acquisition</t>
         </is>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2" s="2" t="n">
         <v>26629895.3</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2" s="2" t="n">
         <v>70799498.06999999</v>
       </c>
       <c r="S2" s="2" t="n">
@@ -1035,7 +1473,7 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="Z2" t="inlineStr">
+      <c r="Z2" s="2" t="inlineStr">
         <is>
           <t>Retained</t>
         </is>
@@ -1061,22 +1499,22 @@
       <c r="AE2" t="n">
         <v>1.75</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2" s="2" t="n">
         <v>50399385.08</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AG2" s="2" t="n">
         <v>95469736.56</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AH2" s="2" t="n">
         <v>59033485.2</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2" s="2" t="n">
         <v>7797067.51</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AJ2" s="2" t="n">
         <v>238515116</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AK2" s="2" t="n">
         <v>34200502.62</v>
       </c>
       <c r="AL2" t="n">
@@ -1108,7 +1546,7 @@
           <t>West Justin</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>AO</t>
         </is>
@@ -1121,7 +1559,7 @@
           <t>E</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>313-51-2957</t>
         </is>
@@ -1146,7 +1584,7 @@
           <t>b10f0d6a-b4ad-405c-9a4f-4f02119be381</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M3" s="2" t="inlineStr">
         <is>
           <t>18-02-2022</t>
         </is>
@@ -1166,15 +1604,16 @@
           <t>Working Capital</t>
         </is>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q3" s="2" t="n">
         <v>55748379.42</v>
       </c>
-      <c r="R3" t="n">
+      <c r="R3" s="2" t="n">
         <v>2783436.06</v>
       </c>
-      <c r="S3" t="n">
+      <c r="S3" s="2" t="n">
         <v>9.76</v>
       </c>
+      <c r="T3" s="2" t="inlineStr"/>
       <c r="U3" t="inlineStr">
         <is>
           <t>Closed</t>
@@ -1195,12 +1634,12 @@
           <t>B</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Y3" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="Z3" t="inlineStr">
+      <c r="Z3" s="2" t="inlineStr">
         <is>
           <t>Retained</t>
         </is>
@@ -1226,22 +1665,22 @@
       <c r="AE3" t="n">
         <v>2</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AF3" s="2" t="n">
         <v>435705344.2</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AG3" s="2" t="n">
         <v>47117668.95</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AH3" s="2" t="n">
         <v>80132376.18000001</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AI3" s="2" t="n">
         <v>7141931.68</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AJ3" s="2" t="n">
         <v>319616293</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="AK3" s="2" t="n">
         <v>156044133.2</v>
       </c>
       <c r="AL3" t="n">
@@ -1286,7 +1725,7 @@
           <t>C</t>
         </is>
       </c>
-      <c r="H4" s="2" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>310-37-1725</t>
         </is>
@@ -1331,16 +1770,16 @@
           <t>Expansion</t>
         </is>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4" s="2" t="n">
         <v>97602997.48</v>
       </c>
-      <c r="R4" t="n">
+      <c r="R4" s="2" t="n">
         <v>80537734.2</v>
       </c>
       <c r="S4" s="2" t="n">
         <v>2.14</v>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="T4" s="2" t="inlineStr">
         <is>
           <t>Equipment</t>
         </is>
@@ -1365,7 +1804,7 @@
           <t>A</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="Y4" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1396,22 +1835,22 @@
       <c r="AE4" t="n">
         <v>2.38</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AF4" s="2" t="n">
         <v>403948022.4</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="AG4" s="2" t="n">
         <v>8926425.41</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AH4" s="2" t="n">
         <v>86863480.34</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AI4" s="2" t="n">
         <v>1955854.73</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AJ4" s="2" t="n">
         <v>451241665.5</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AK4" s="2" t="n">
         <v>160851816.4</v>
       </c>
       <c r="AL4" t="n">
@@ -1456,7 +1895,7 @@
           <t>E</t>
         </is>
       </c>
-      <c r="H5" s="2" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>447-80-2607</t>
         </is>
@@ -1481,12 +1920,12 @@
           <t>d101c317-a06e-4a8f-8e63-d921c33b1a59</t>
         </is>
       </c>
-      <c r="M5" s="2" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>26-08-2023</t>
         </is>
       </c>
-      <c r="N5" s="2" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>19-11-2029</t>
         </is>
@@ -1501,16 +1940,16 @@
           <t>Expansion</t>
         </is>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q5" s="2" t="n">
         <v>19714396.46</v>
       </c>
-      <c r="R5" t="n">
+      <c r="R5" s="2" t="n">
         <v>39263759.32</v>
       </c>
-      <c r="S5" t="n">
+      <c r="S5" s="2" t="n">
         <v>2.9</v>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="T5" s="2" t="inlineStr">
         <is>
           <t>Real Estate</t>
         </is>
@@ -1535,7 +1974,7 @@
           <t>CCC</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr">
+      <c r="Y5" s="2" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
@@ -1566,22 +2005,22 @@
       <c r="AE5" t="n">
         <v>2.9</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AF5" s="2" t="n">
         <v>92416015.06</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AG5" s="2" t="n">
         <v>213720317.6</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AH5" s="2" t="n">
         <v>59098537.91</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AI5" s="2" t="n">
         <v>6667902.48</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AJ5" s="2" t="n">
         <v>22780570.2</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="AK5" s="2" t="n">
         <v>100793798.8</v>
       </c>
       <c r="AL5" t="n">
@@ -1626,7 +2065,7 @@
           <t>A</t>
         </is>
       </c>
-      <c r="H6" s="2" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>705-09-9417</t>
         </is>
@@ -1671,16 +2110,16 @@
           <t>Refinancing</t>
         </is>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q6" s="2" t="n">
         <v>17232454.13</v>
       </c>
-      <c r="R6" t="n">
+      <c r="R6" s="2" t="n">
         <v>86223792.98999999</v>
       </c>
-      <c r="S6" t="n">
+      <c r="S6" s="2" t="n">
         <v>8.9</v>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="T6" s="2" t="inlineStr">
         <is>
           <t>Equipment</t>
         </is>
@@ -1705,7 +2144,7 @@
           <t>BB</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
+      <c r="Y6" s="2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1736,22 +2175,22 @@
       <c r="AE6" t="n">
         <v>2.52</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AF6" s="2" t="n">
         <v>133472482.2</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="AG6" s="2" t="n">
         <v>294279690.6</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="AH6" s="2" t="n">
         <v>70419654.54000001</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AI6" s="2" t="n">
         <v>4335752.01</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="AJ6" s="2" t="n">
         <v>391850032.4</v>
       </c>
-      <c r="AK6" t="n">
+      <c r="AK6" s="2" t="n">
         <v>123734826.9</v>
       </c>
       <c r="AL6" t="n">
@@ -1783,7 +2222,7 @@
           <t>Martinfort</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>IS</t>
         </is>
@@ -1841,16 +2280,16 @@
           <t>Refinancing</t>
         </is>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7" s="2" t="n">
         <v>15850912.22</v>
       </c>
-      <c r="R7" t="n">
+      <c r="R7" s="2" t="n">
         <v>76069643.34999999</v>
       </c>
       <c r="S7" s="2" t="n">
         <v>10.18</v>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="T7" s="2" t="inlineStr">
         <is>
           <t>Real Estate</t>
         </is>
@@ -1875,7 +2314,7 @@
           <t>CCC</t>
         </is>
       </c>
-      <c r="Y7" t="inlineStr">
+      <c r="Y7" s="2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1906,25 +2345,25 @@
       <c r="AE7" t="n">
         <v>2.86</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AF7" s="2" t="n">
         <v>395983983</v>
       </c>
-      <c r="AG7" t="n">
+      <c r="AG7" s="2" t="n">
         <v>62424518.88</v>
       </c>
-      <c r="AH7" t="n">
+      <c r="AH7" s="2" t="n">
         <v>80765395.66</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AI7" s="2" t="n">
         <v>38633214.12</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AJ7" s="2" t="n">
         <v>357587093</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="AK7" s="2" t="n">
         <v>40729410.51</v>
       </c>
-      <c r="AL7" t="n">
+      <c r="AL7" s="2" t="n">
         <v>10211446.33</v>
       </c>
       <c r="AM7" t="n">
@@ -1958,7 +2397,7 @@
           <t>BA</t>
         </is>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" t="n">
         <v>6197</v>
       </c>
       <c r="G8" t="inlineStr">
@@ -1966,7 +2405,7 @@
           <t>D</t>
         </is>
       </c>
-      <c r="H8" s="2" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>418-76-6498</t>
         </is>
@@ -1981,7 +2420,7 @@
           <t>hiq</t>
         </is>
       </c>
-      <c r="K8" s="2" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>JtrGcv</t>
         </is>
@@ -2011,10 +2450,10 @@
           <t>Working Capital</t>
         </is>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8" s="2" t="n">
         <v>36787659.22</v>
       </c>
-      <c r="R8" t="n">
+      <c r="R8" s="2" t="n">
         <v>73539555.18000001</v>
       </c>
       <c r="S8" s="2" t="n">
@@ -2076,25 +2515,25 @@
       <c r="AE8" t="n">
         <v>1.22</v>
       </c>
-      <c r="AF8" t="n">
+      <c r="AF8" s="2" t="n">
         <v>66196202.67</v>
       </c>
-      <c r="AG8" t="n">
+      <c r="AG8" s="2" t="n">
         <v>355967893</v>
       </c>
-      <c r="AH8" t="n">
+      <c r="AH8" s="2" t="n">
         <v>99485689.37</v>
       </c>
-      <c r="AI8" t="n">
+      <c r="AI8" s="2" t="n">
         <v>12237839.84</v>
       </c>
-      <c r="AJ8" t="n">
+      <c r="AJ8" s="2" t="n">
         <v>337813878.6</v>
       </c>
-      <c r="AK8" t="n">
+      <c r="AK8" s="2" t="n">
         <v>78824972.5</v>
       </c>
-      <c r="AL8" t="n">
+      <c r="AL8" s="2" t="n">
         <v>13252269.4</v>
       </c>
       <c r="AM8" t="n">
@@ -2128,7 +2567,7 @@
           <t>BE</t>
         </is>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" t="n">
         <v>7922</v>
       </c>
       <c r="G9" t="inlineStr">
@@ -2136,7 +2575,7 @@
           <t>D</t>
         </is>
       </c>
-      <c r="H9" s="2" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>617-78-1101</t>
         </is>
@@ -2151,7 +2590,7 @@
           <t>jdE</t>
         </is>
       </c>
-      <c r="K9" s="2" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>YaJkhL</t>
         </is>
@@ -2181,15 +2620,16 @@
           <t>Refinancing</t>
         </is>
       </c>
-      <c r="Q9" t="n">
+      <c r="Q9" s="2" t="n">
         <v>98519519.33</v>
       </c>
-      <c r="R9" t="n">
+      <c r="R9" s="2" t="n">
         <v>83846458.68000001</v>
       </c>
-      <c r="S9" t="n">
+      <c r="S9" s="2" t="n">
         <v>6.55</v>
       </c>
+      <c r="T9" s="2" t="inlineStr"/>
       <c r="U9" t="inlineStr">
         <is>
           <t>Defaulted</t>
@@ -2241,22 +2681,22 @@
       <c r="AE9" t="n">
         <v>1.43</v>
       </c>
-      <c r="AF9" t="n">
+      <c r="AF9" s="2" t="n">
         <v>58823388.81</v>
       </c>
-      <c r="AG9" t="n">
+      <c r="AG9" s="2" t="n">
         <v>267077344.9</v>
       </c>
-      <c r="AH9" t="n">
+      <c r="AH9" s="2" t="n">
         <v>30948149.11</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AI9" s="2" t="n">
         <v>1559826.73</v>
       </c>
-      <c r="AJ9" t="n">
+      <c r="AJ9" s="2" t="n">
         <v>309303560</v>
       </c>
-      <c r="AK9" t="n">
+      <c r="AK9" s="2" t="n">
         <v>41207930.04</v>
       </c>
       <c r="AL9" t="n">

</xml_diff>